<commit_message>
small fixes monograms added auxiliary removed enter,focus added spanish filter added ser (skiprow) fixed
</commit_message>
<xml_diff>
--- a/verbos.xlsx
+++ b/verbos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DUE\Python\Conjugador6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84DB66F-555E-4260-A27A-E744BDF21D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D74BB9-65EE-49C7-9A9C-39695C6C4B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23865" yWindow="0" windowWidth="14640" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verbos" sheetId="6" r:id="rId1"/>
@@ -20887,10 +20887,10 @@
   <dimension ref="A1:S290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C240" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C134" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="A291" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>